<commit_message>
fix list student in grade default file
</commit_message>
<xml_diff>
--- a/server/uploads/files/list-students-upload.xlsx
+++ b/server/uploads/files/list-students-upload.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A08700-5084-4367-A9E4-08293C94372E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7ABD673-279B-4A27-9182-E721B281CF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="456" windowWidth="17280" windowHeight="11784" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet 1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>StudendId</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t>Nguyễn Thanh Tùng</t>
+  </si>
+  <si>
+    <t>Nguyển Văn A</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,6 +470,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>20120600</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>

</xml_diff>